<commit_message>
[Silverfox] Mob - FX Data, Asset 등
</commit_message>
<xml_diff>
--- a/DesignDocs/빌드 통합 관리.xlsx
+++ b/DesignDocs/빌드 통합 관리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3492097C-8CC1-4336-92D6-47A7F1AD50D6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFD6738-3541-479E-8A5D-8368C4381773}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{434CAAA1-D6EA-4AF4-BB0C-824F397259BA}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$52</definedName>
   </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="109">
   <si>
     <t>순번</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -377,6 +377,45 @@
   </si>
   <si>
     <t>NPC - NPC가 피격 되었을 때 뒤로 살짝 물러나게 하는 구조에 관한 문서 작성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>042</t>
+  </si>
+  <si>
+    <t>043</t>
+  </si>
+  <si>
+    <t>044</t>
+  </si>
+  <si>
+    <t>045</t>
+  </si>
+  <si>
+    <t>046</t>
+  </si>
+  <si>
+    <t>047</t>
+  </si>
+  <si>
+    <t>048</t>
+  </si>
+  <si>
+    <t>049</t>
+  </si>
+  <si>
+    <t>050</t>
+  </si>
+  <si>
+    <t>NPC - NPC가 스킬의 유형이 2가지 이상 가지고 있을 때 Idle/Walk의 상태 변환에 관한 규칙 생성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>051</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - NPC의 Animaion Sprite에서 데미지 플로팅 Event 추가하기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -775,17 +814,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5FF190-EDCE-43C7-A5C3-EF5175D3AC25}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.25" customWidth="1"/>
-    <col min="3" max="3" width="56.375" customWidth="1"/>
+    <col min="3" max="3" width="91.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.875" customWidth="1"/>
     <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
@@ -1219,6 +1258,9 @@
       <c r="C34" t="s">
         <v>75</v>
       </c>
+      <c r="D34">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
@@ -1238,6 +1280,9 @@
       <c r="C36" t="s">
         <v>77</v>
       </c>
+      <c r="D36">
+        <v>0.04</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
@@ -1304,52 +1349,131 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="C43" t="s">
         <v>88</v>
       </c>
+      <c r="D43">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>98</v>
+      </c>
       <c r="C44" t="s">
         <v>89</v>
       </c>
+      <c r="D44">
+        <v>0.02</v>
+      </c>
+      <c r="E44" s="4">
+        <v>43322</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="C45" t="s">
         <v>90</v>
       </c>
+      <c r="D45">
+        <v>0.02</v>
+      </c>
+      <c r="E45" s="4">
+        <v>43322</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="C46" t="s">
         <v>91</v>
       </c>
+      <c r="D46">
+        <v>0.02</v>
+      </c>
+      <c r="E46" s="4">
+        <v>43322</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>101</v>
+      </c>
       <c r="C47" t="s">
         <v>92</v>
       </c>
+      <c r="D47">
+        <v>0.02</v>
+      </c>
+      <c r="E47" s="4">
+        <v>43322</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="C48" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D48">
+        <v>0.02</v>
+      </c>
+      <c r="E48" s="4">
+        <v>43322</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="C49" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="D49">
+        <v>0.02</v>
+      </c>
+      <c r="E49" s="4">
+        <v>43322</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="C50" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>105</v>
+      </c>
       <c r="C51" t="s">
         <v>96</v>
       </c>
     </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>108</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F37" xr:uid="{F15FEA23-80D4-4682-8C45-8A0EDFA6E03B}"/>
+  <autoFilter ref="A1:F52" xr:uid="{F15FEA23-80D4-4682-8C45-8A0EDFA6E03B}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Silverfox] Owl 관련 NPC 기본 적용
</commit_message>
<xml_diff>
--- a/DesignDocs/빌드 통합 관리.xlsx
+++ b/DesignDocs/빌드 통합 관리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2D-Side-View-Roguelike\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C4D5C7C-86B8-46E1-BD45-BBA54A71B1FA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4B803D-3318-48DA-8973-B86ADD8A216F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{434CAAA1-D6EA-4AF4-BB0C-824F397259BA}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="144">
   <si>
     <t>순번</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -51,10 +51,6 @@
   </si>
   <si>
     <t>001</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>유형</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -493,6 +489,63 @@
   </si>
   <si>
     <t>067</t>
+  </si>
+  <si>
+    <t>UI - 인게임에서 외곽 주변이 뿌옇게 보이는 현상</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI - 세팅된 스킬 사라지지 않게 하기</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI - 튜토리얼 구성</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - 기본 이동 처리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - 복귀 처리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - 복귀 불가시 배회처리</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NPC - 인식 종료</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC - PC의 FX 피봇 위치 설정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC - PC의 Fx Prefab 재 설정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range/Bounce를 Default값으로 두어 Melee를 예외처리 한다.
+이때, Melee를 보유 / 중복 보유 하고 있는 경우 공격 후 Move처리 한다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>인호</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>상현</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PC - Style Data에서 Pivot 설정 하는 방법</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>담당자</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -532,7 +585,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
@@ -592,13 +645,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -918,7 +971,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -929,7 +982,7 @@
     <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.875" customWidth="1"/>
     <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.625" customWidth="1"/>
+    <col min="7" max="7" width="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -937,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>143</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -952,7 +1005,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -961,7 +1014,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>0.01</v>
@@ -975,10 +1028,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <v>0.01</v>
@@ -992,10 +1045,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>0.03</v>
@@ -1003,23 +1056,23 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="7">
+        <v>38</v>
+      </c>
+      <c r="D5" s="6">
         <v>0.03</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="8">
+        <v>39</v>
+      </c>
+      <c r="D6" s="7">
         <v>0.02</v>
       </c>
       <c r="E6" s="4">
@@ -1031,10 +1084,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <v>0.01</v>
@@ -1048,10 +1101,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8">
         <v>0.01</v>
@@ -1065,10 +1118,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9">
         <v>0.01</v>
@@ -1082,10 +1135,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>0.01</v>
@@ -1099,10 +1152,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D11">
         <v>0.01</v>
@@ -1116,10 +1169,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <v>0.01</v>
@@ -1133,10 +1186,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13">
         <v>0.03</v>
@@ -1144,10 +1197,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>0.04</v>
@@ -1158,10 +1211,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D15">
         <v>0.01</v>
@@ -1175,10 +1228,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16">
         <v>0.05</v>
@@ -1186,10 +1239,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17">
         <v>0.05</v>
@@ -1197,18 +1250,18 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19">
         <v>0.01</v>
@@ -1222,10 +1275,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20">
         <v>0.02</v>
@@ -1239,10 +1292,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D21">
         <v>0.03</v>
@@ -1250,10 +1303,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22">
         <v>0.02</v>
@@ -1267,10 +1320,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23">
         <v>0.02</v>
@@ -1284,10 +1337,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D24">
         <v>0.03</v>
@@ -1295,10 +1348,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D25">
         <v>0.03</v>
@@ -1306,10 +1359,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26">
         <v>0.05</v>
@@ -1317,10 +1370,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27">
         <v>0.06</v>
@@ -1328,10 +1381,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28">
         <v>7.0000000000000007E-2</v>
@@ -1339,10 +1392,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29">
         <v>0.05</v>
@@ -1350,18 +1403,18 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D31">
         <v>0.02</v>
@@ -1375,10 +1428,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D32">
         <v>0.02</v>
@@ -1392,10 +1445,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D33">
         <v>0.03</v>
@@ -1403,10 +1456,10 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D34">
         <v>0.04</v>
@@ -1414,10 +1467,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D35">
         <v>0.03</v>
@@ -1425,10 +1478,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D36">
         <v>0.04</v>
@@ -1436,10 +1489,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D37">
         <v>0.02</v>
@@ -1447,10 +1500,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D38">
         <v>0.03</v>
@@ -1459,10 +1512,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D39">
         <v>0.03</v>
@@ -1470,10 +1523,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D40">
         <v>0.01</v>
@@ -1481,10 +1534,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D41">
         <v>0.02</v>
@@ -1492,10 +1545,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D42">
         <v>0.03</v>
@@ -1503,10 +1556,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C43" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D43">
         <v>0.02</v>
@@ -1514,10 +1567,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D44">
         <v>0.02</v>
@@ -1531,10 +1584,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D45">
         <v>0.02</v>
@@ -1548,10 +1601,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D46">
         <v>0.02</v>
@@ -1565,10 +1618,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D47">
         <v>0.02</v>
@@ -1582,10 +1635,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D48">
         <v>0.02</v>
@@ -1599,10 +1652,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D49">
         <v>0.02</v>
@@ -1616,125 +1669,187 @@
     </row>
     <row r="50" spans="1:7" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
+      </c>
+      <c r="B50" t="s">
+        <v>140</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B51" t="s">
+        <v>141</v>
+      </c>
+      <c r="C51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="66" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B52" t="s">
+        <v>140</v>
+      </c>
+      <c r="C52" t="s">
         <v>105</v>
       </c>
-      <c r="C51" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52" t="s">
-        <v>106</v>
+      <c r="G52" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="B53" t="s">
+        <v>141</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+      <c r="B54" t="s">
+        <v>141</v>
       </c>
       <c r="C54" t="s">
-        <v>113</v>
+        <v>112</v>
+      </c>
+      <c r="D54">
+        <v>0.05</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" t="s">
         <v>115</v>
-      </c>
-      <c r="C55" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C58" s="6"/>
+        <v>119</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="C59" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="C60" t="s">
+        <v>133</v>
+      </c>
+      <c r="D60">
+        <v>0.05</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
+      </c>
+      <c r="C61" t="s">
+        <v>134</v>
+      </c>
+      <c r="D61">
+        <v>0.05</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
+      </c>
+      <c r="C62" t="s">
+        <v>135</v>
+      </c>
+      <c r="D62">
+        <v>0.05</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
+      </c>
+      <c r="C63" t="s">
+        <v>136</v>
+      </c>
+      <c r="D63">
+        <v>0.05</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
+      <c r="C65" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
+      <c r="C66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>